<commit_message>
new test cases added for unit and collection
</commit_message>
<xml_diff>
--- a/src/test/resources/excel/unit.xlsx
+++ b/src/test/resources/excel/unit.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\code\selenium-testng\jioFabricAutomation\src\test\resources\excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A41549F1-4AB9-4AE8-AB0E-6BE7B882B4E3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EAEC26A0-4092-464D-AD90-D1C0ED51C13B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13140" xr2:uid="{04E55122-9D7C-482F-A624-2D17462FB4FA}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13140" activeTab="1" xr2:uid="{04E55122-9D7C-482F-A624-2D17462FB4FA}"/>
   </bookViews>
   <sheets>
     <sheet name="Unit" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="190" uniqueCount="83">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="194" uniqueCount="84">
   <si>
     <t>name</t>
   </si>
@@ -245,9 +245,6 @@
     <t>medium</t>
   </si>
   <si>
-    <t>score</t>
-  </si>
-  <si>
     <t>dgfgyh</t>
   </si>
   <si>
@@ -257,12 +254,6 @@
     <t>m1,m2,m3</t>
   </si>
   <si>
-    <t>entity</t>
-  </si>
-  <si>
-    <t>order</t>
-  </si>
-  <si>
     <t>first</t>
   </si>
   <si>
@@ -282,13 +273,117 @@
   </si>
   <si>
     <t>valueType</t>
+  </si>
+  <si>
+    <t>filePath</t>
+  </si>
+  <si>
+    <r>
+      <t>C:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9.8000000000000007"/>
+        <color rgb="FFCC7832"/>
+        <rFont val="JetBrains Mono"/>
+        <family val="3"/>
+      </rPr>
+      <t>\\</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9.8000000000000007"/>
+        <color rgb="FF6A8759"/>
+        <rFont val="JetBrains Mono"/>
+        <family val="3"/>
+      </rPr>
+      <t>Users</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9.8000000000000007"/>
+        <color rgb="FFCC7832"/>
+        <rFont val="JetBrains Mono"/>
+        <family val="3"/>
+      </rPr>
+      <t>\\</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9.8000000000000007"/>
+        <color rgb="FF6A8759"/>
+        <rFont val="JetBrains Mono"/>
+        <family val="3"/>
+      </rPr>
+      <t>dell</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9.8000000000000007"/>
+        <color rgb="FFCC7832"/>
+        <rFont val="JetBrains Mono"/>
+        <family val="3"/>
+      </rPr>
+      <t>\\</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9.8000000000000007"/>
+        <color rgb="FF6A8759"/>
+        <rFont val="JetBrains Mono"/>
+        <family val="3"/>
+      </rPr>
+      <t>Desktop</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9.8000000000000007"/>
+        <color rgb="FFCC7832"/>
+        <rFont val="JetBrains Mono"/>
+        <family val="3"/>
+      </rPr>
+      <t>\\</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9.8000000000000007"/>
+        <color rgb="FF6A8759"/>
+        <rFont val="JetBrains Mono"/>
+        <family val="3"/>
+      </rPr>
+      <t>New_Json</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9.8000000000000007"/>
+        <color rgb="FFCC7832"/>
+        <rFont val="JetBrains Mono"/>
+        <family val="3"/>
+      </rPr>
+      <t>\\</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9.8000000000000007"/>
+        <color rgb="FF6A8759"/>
+        <rFont val="JetBrains Mono"/>
+        <family val="3"/>
+      </rPr>
+      <t>unitConfigSample.json</t>
+    </r>
+  </si>
+  <si>
+    <t>C:\\Users\\dell\\Desktop\\New_Json\\collectionSample.json</t>
+  </si>
+  <si>
+    <t>main</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="5">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -306,6 +401,18 @@
       <sz val="9"/>
       <color rgb="FF202124"/>
       <name val="Consolas"/>
+      <family val="3"/>
+    </font>
+    <font>
+      <sz val="9.8000000000000007"/>
+      <color rgb="FF6A8759"/>
+      <name val="JetBrains Mono"/>
+      <family val="3"/>
+    </font>
+    <font>
+      <sz val="9.8000000000000007"/>
+      <color rgb="FFCC7832"/>
+      <name val="JetBrains Mono"/>
       <family val="3"/>
     </font>
   </fonts>
@@ -329,10 +436,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -647,13 +757,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{10F12242-BA7E-4D49-851F-EEF3D4B7879B}">
-  <dimension ref="A1:R12"/>
+  <dimension ref="A1:S12"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="Q22" sqref="Q22"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="N17" sqref="N17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="16.140625" customWidth="1"/>
     <col min="2" max="5" width="14.28515625" customWidth="1"/>
@@ -666,9 +776,10 @@
     <col min="16" max="16" width="12" customWidth="1"/>
     <col min="17" max="17" width="14" customWidth="1"/>
     <col min="18" max="18" width="12.5703125" customWidth="1"/>
+    <col min="19" max="19" width="19.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:19">
       <c r="A1" t="s">
         <v>2</v>
       </c>
@@ -718,18 +829,21 @@
         <v>41</v>
       </c>
       <c r="Q1" t="s">
+        <v>76</v>
+      </c>
+      <c r="R1" t="s">
         <v>79</v>
       </c>
-      <c r="R1" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="2" spans="1:18" ht="16.5" x14ac:dyDescent="0.3">
+      <c r="S1" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="2" spans="1:19" ht="16.5">
       <c r="A2" t="s">
         <v>3</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="C2" t="s">
         <v>60</v>
@@ -765,10 +879,13 @@
         <v>62</v>
       </c>
       <c r="P2" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="3" spans="1:18" x14ac:dyDescent="0.25">
+        <v>39</v>
+      </c>
+      <c r="S2" s="3" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="3" spans="1:19">
       <c r="A3" t="s">
         <v>4</v>
       </c>
@@ -803,7 +920,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="4" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:19">
       <c r="A4" t="s">
         <v>28</v>
       </c>
@@ -838,7 +955,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="5" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:19">
       <c r="A5" t="s">
         <v>6</v>
       </c>
@@ -873,7 +990,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="6" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:19">
       <c r="A6" t="s">
         <v>7</v>
       </c>
@@ -908,7 +1025,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="7" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:19">
       <c r="A7" t="s">
         <v>8</v>
       </c>
@@ -943,7 +1060,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="8" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:19">
       <c r="A8" t="s">
         <v>9</v>
       </c>
@@ -978,7 +1095,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="9" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:19">
       <c r="A9" t="s">
         <v>10</v>
       </c>
@@ -1013,7 +1130,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="10" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:19">
       <c r="A10" t="s">
         <v>11</v>
       </c>
@@ -1048,18 +1165,18 @@
         <v>40</v>
       </c>
     </row>
-    <row r="11" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:19">
       <c r="A11" t="s">
         <v>12</v>
       </c>
       <c r="B11" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="D11" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="I11" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="N11" t="s">
         <v>43</v>
@@ -1068,16 +1185,16 @@
         <v>5</v>
       </c>
       <c r="P11" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="Q11" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="R11" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="12" spans="1:18" x14ac:dyDescent="0.25">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="12" spans="1:19">
       <c r="A12" t="s">
         <v>13</v>
       </c>
@@ -1120,21 +1237,22 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C1063F3A-212E-4807-A35D-358B161F4624}">
-  <dimension ref="A1:G12"/>
+  <dimension ref="A1:H12"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G16" sqref="G16"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H21" sqref="H21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="2" width="16" customWidth="1"/>
     <col min="4" max="5" width="15.7109375" customWidth="1"/>
     <col min="6" max="6" width="20.42578125" customWidth="1"/>
     <col min="7" max="7" width="16.42578125" customWidth="1"/>
+    <col min="8" max="8" width="57.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8">
       <c r="A1" t="s">
         <v>2</v>
       </c>
@@ -1151,21 +1269,24 @@
         <v>48</v>
       </c>
       <c r="F1" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="G1" t="s">
         <v>41</v>
       </c>
-    </row>
-    <row r="2" spans="1:7" ht="16.5" x14ac:dyDescent="0.3">
+      <c r="H1" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" ht="16.5">
       <c r="A2" t="s">
         <v>3</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>74</v>
+        <v>63</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>70</v>
+        <v>83</v>
       </c>
       <c r="D2" t="s">
         <v>64</v>
@@ -1174,13 +1295,16 @@
         <v>65</v>
       </c>
       <c r="F2" t="s">
-        <v>75</v>
+        <v>83</v>
       </c>
       <c r="G2" t="s">
         <v>39</v>
       </c>
-    </row>
-    <row r="3" spans="1:7" ht="16.5" x14ac:dyDescent="0.3">
+      <c r="H2" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" ht="16.5">
       <c r="A3" t="s">
         <v>4</v>
       </c>
@@ -1197,7 +1321,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="4" spans="1:7" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:8" ht="16.5">
       <c r="A4" t="s">
         <v>28</v>
       </c>
@@ -1205,13 +1329,13 @@
         <v>63</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="G4" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:8">
       <c r="A5" t="s">
         <v>6</v>
       </c>
@@ -1225,13 +1349,13 @@
         <v>68</v>
       </c>
       <c r="E5" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="G5" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:8">
       <c r="A6" t="s">
         <v>7</v>
       </c>
@@ -1242,7 +1366,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:8">
       <c r="A7" t="s">
         <v>8</v>
       </c>
@@ -1253,7 +1377,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:8">
       <c r="A8" t="s">
         <v>9</v>
       </c>
@@ -1264,7 +1388,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:8">
       <c r="A9" t="s">
         <v>10</v>
       </c>
@@ -1275,7 +1399,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:8">
       <c r="A10" t="s">
         <v>11</v>
       </c>
@@ -1286,7 +1410,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:8">
       <c r="A11" t="s">
         <v>12</v>
       </c>
@@ -1297,7 +1421,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:8">
       <c r="A12" t="s">
         <v>13</v>
       </c>

</xml_diff>